<commit_message>
Changes to be committed: 	modified:   Results/combined_data.xlsx 	modified:   VRU Headform
</commit_message>
<xml_diff>
--- a/Results/combined_data.xlsx
+++ b/Results/combined_data.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -491,6 +496,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -505,6 +513,9 @@
       <c r="D3" t="n">
         <v>9</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.0371900826446281</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -519,6 +530,9 @@
       <c r="D4" t="n">
         <v>77.25</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.4256198347107438</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -533,6 +547,9 @@
       <c r="D5" t="n">
         <v>32.5</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.268595041322314</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -547,6 +564,9 @@
       <c r="D6" t="n">
         <v>2.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.04132231404958678</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -561,6 +581,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.1694214876033058</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -575,6 +598,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.05785123966942149</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -587,6 +613,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -600,6 +629,9 @@
       </c>
       <c r="D10" t="n">
         <v>121.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -613,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -638,6 +670,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -652,6 +689,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -666,6 +706,9 @@
       <c r="D3" t="n">
         <v>79</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.3434782608695652</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -680,6 +723,9 @@
       <c r="D4" t="n">
         <v>60.75</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.3521739130434783</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -694,6 +740,9 @@
       <c r="D5" t="n">
         <v>13.5</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1173913043478261</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -708,6 +757,9 @@
       <c r="D6" t="n">
         <v>2.25</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.0391304347826087</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -722,6 +774,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.09565217391304348</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -736,6 +791,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.05217391304347826</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -748,6 +806,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -761,6 +822,9 @@
       </c>
       <c r="D10" t="n">
         <v>155.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -774,7 +838,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -799,6 +863,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -813,6 +882,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -827,6 +899,9 @@
       <c r="D3" t="n">
         <v>95</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.3830645161290323</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -841,6 +916,9 @@
       <c r="D4" t="n">
         <v>56.25</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.3024193548387097</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -855,6 +933,9 @@
       <c r="D5" t="n">
         <v>13</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1048387096774194</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -869,6 +950,9 @@
       <c r="D6" t="n">
         <v>3</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.04838709677419355</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -883,6 +967,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.1209677419354839</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -897,6 +984,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.04032258064516129</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -909,6 +999,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -922,6 +1015,9 @@
       </c>
       <c r="D10" t="n">
         <v>167.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -935,7 +1031,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -960,6 +1056,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -974,6 +1075,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -988,6 +1092,9 @@
       <c r="D3" t="n">
         <v>51</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.1976744186046512</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -1002,6 +1109,9 @@
       <c r="D4" t="n">
         <v>76.5</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.3953488372093023</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -1016,6 +1126,9 @@
       <c r="D5" t="n">
         <v>18.5</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1434108527131783</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -1030,6 +1143,9 @@
       <c r="D6" t="n">
         <v>4.25</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.06589147286821706</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -1044,6 +1160,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.1356589147286822</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -1058,6 +1177,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.06201550387596899</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -1070,6 +1192,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1083,6 +1208,9 @@
       </c>
       <c r="D10" t="n">
         <v>150.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1096,7 +1224,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1121,6 +1249,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -1135,6 +1268,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -1149,6 +1285,9 @@
       <c r="D3" t="n">
         <v>72</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.2790697674418605</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -1163,6 +1302,9 @@
       <c r="D4" t="n">
         <v>48.75</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.251937984496124</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -1177,6 +1319,9 @@
       <c r="D5" t="n">
         <v>23</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1782945736434109</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -1191,6 +1336,9 @@
       <c r="D6" t="n">
         <v>4.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.06976744186046512</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -1205,6 +1353,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.189922480620155</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -1219,6 +1370,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.0310077519379845</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -1231,6 +1385,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1244,6 +1401,9 @@
       </c>
       <c r="D10" t="n">
         <v>148.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1257,7 +1417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1282,6 +1442,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -1296,6 +1461,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -1310,6 +1478,9 @@
       <c r="D3" t="n">
         <v>92</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -1324,6 +1495,9 @@
       <c r="D4" t="n">
         <v>44.25</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.2565217391304348</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -1338,6 +1512,9 @@
       <c r="D5" t="n">
         <v>17</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1478260869565217</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -1352,6 +1529,9 @@
       <c r="D6" t="n">
         <v>5.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.09565217391304348</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -1366,6 +1546,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.04782608695652174</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -1380,6 +1563,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.05217391304347826</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -1392,6 +1578,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1405,6 +1594,9 @@
       </c>
       <c r="D10" t="n">
         <v>158.75</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1418,7 +1610,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1443,6 +1635,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -1457,6 +1654,9 @@
       <c r="D2" t="n">
         <v>20</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.08264462809917356</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -1471,6 +1671,9 @@
       <c r="D3" t="n">
         <v>32</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.1322314049586777</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -1485,6 +1688,9 @@
       <c r="D4" t="n">
         <v>65.25</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.359504132231405</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -1499,6 +1705,9 @@
       <c r="D5" t="n">
         <v>23</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1900826446280992</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -1513,6 +1722,9 @@
       <c r="D6" t="n">
         <v>3.75</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.06198347107438017</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -1527,6 +1739,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.08264462809917356</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -1541,6 +1756,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.05785123966942149</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -1553,6 +1771,9 @@
         <v>8</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0.03305785123966942</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1566,6 +1787,9 @@
       </c>
       <c r="D10" t="n">
         <v>144</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1579,7 +1803,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1604,6 +1828,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -1618,6 +1847,9 @@
       <c r="D2" t="n">
         <v>15</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.05952380952380952</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -1632,6 +1864,9 @@
       <c r="D3" t="n">
         <v>70</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.2777777777777778</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -1646,6 +1881,9 @@
       <c r="D4" t="n">
         <v>37.5</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.1984126984126984</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -1660,6 +1898,9 @@
       <c r="D5" t="n">
         <v>15.5</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.123015873015873</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -1674,6 +1915,9 @@
       <c r="D6" t="n">
         <v>8.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.1349206349206349</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -1688,6 +1932,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.1666666666666667</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -1702,6 +1949,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.03968253968253968</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -1714,6 +1964,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1727,6 +1980,9 @@
       </c>
       <c r="D10" t="n">
         <v>146.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9999999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1740,7 +1996,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1765,6 +2021,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -1779,6 +2040,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -1793,6 +2057,9 @@
       <c r="D3" t="n">
         <v>53</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.2304347826086957</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -1807,6 +2074,9 @@
       <c r="D4" t="n">
         <v>81.75</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.4739130434782609</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -1821,6 +2091,9 @@
       <c r="D5" t="n">
         <v>9</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.0782608695652174</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -1835,6 +2108,9 @@
       <c r="D6" t="n">
         <v>5.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.09565217391304348</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -1849,6 +2125,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.06086956521739131</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -1863,6 +2142,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.06086956521739131</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -1875,6 +2157,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1888,6 +2173,9 @@
       </c>
       <c r="D10" t="n">
         <v>149.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9999999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1901,7 +2189,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1926,6 +2214,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -1940,6 +2233,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -1954,6 +2250,9 @@
       <c r="D3" t="n">
         <v>29</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -1968,6 +2267,9 @@
       <c r="D4" t="n">
         <v>75.75</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.4353448275862069</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -1982,6 +2284,9 @@
       <c r="D5" t="n">
         <v>22</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1896551724137931</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -1996,6 +2301,9 @@
       <c r="D6" t="n">
         <v>5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.08620689655172414</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -2010,6 +2318,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.1120689655172414</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -2024,6 +2335,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.05172413793103448</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -2036,6 +2350,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2049,6 +2366,9 @@
       </c>
       <c r="D10" t="n">
         <v>131.75</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2062,7 +2382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2087,6 +2407,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -2101,6 +2426,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -2115,6 +2443,9 @@
       <c r="D3" t="n">
         <v>37</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.1594827586206897</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -2129,6 +2460,9 @@
       <c r="D4" t="n">
         <v>108.75</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.625</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -2143,6 +2477,9 @@
       <c r="D5" t="n">
         <v>10</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.08620689655172414</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -2157,6 +2494,9 @@
       <c r="D6" t="n">
         <v>2.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.04310344827586207</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -2171,6 +2511,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.03448275862068965</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -2185,6 +2528,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.05172413793103448</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -2197,6 +2543,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2210,6 +2559,9 @@
       </c>
       <c r="D10" t="n">
         <v>158.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2223,7 +2575,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2248,6 +2600,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -2262,6 +2619,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -2276,6 +2636,9 @@
       <c r="D3" t="n">
         <v>29</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.1150793650793651</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -2290,6 +2653,9 @@
       <c r="D4" t="n">
         <v>55.5</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.2936507936507937</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -2304,6 +2670,9 @@
       <c r="D5" t="n">
         <v>28</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.2222222222222222</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -2318,6 +2687,9 @@
       <c r="D6" t="n">
         <v>6.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.1031746031746032</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -2332,6 +2704,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.2420634920634921</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -2346,6 +2721,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.02380952380952381</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -2358,6 +2736,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2371,6 +2752,9 @@
       </c>
       <c r="D10" t="n">
         <v>119</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2384,7 +2768,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2409,6 +2793,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -2423,6 +2812,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -2437,6 +2829,9 @@
       <c r="D3" t="n">
         <v>96</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.5581395348837209</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -2451,6 +2846,9 @@
       <c r="D4" t="n">
         <v>26.25</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.2034883720930233</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -2465,6 +2863,9 @@
       <c r="D5" t="n">
         <v>10</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1162790697674419</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -2479,6 +2880,9 @@
       <c r="D6" t="n">
         <v>2</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.04651162790697674</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -2493,6 +2897,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.05232558139534884</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -2507,6 +2914,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.02325581395348837</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -2519,6 +2929,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2532,6 +2945,9 @@
       </c>
       <c r="D10" t="n">
         <v>134.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2545,7 +2961,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2570,6 +2986,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -2584,6 +3005,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -2598,6 +3022,9 @@
       <c r="D3" t="n">
         <v>32</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.1904761904761905</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -2612,6 +3039,9 @@
       <c r="D4" t="n">
         <v>32.25</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.2559523809523809</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -2626,6 +3056,9 @@
       <c r="D5" t="n">
         <v>26</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.3095238095238095</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -2640,6 +3073,9 @@
       <c r="D6" t="n">
         <v>4.25</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.1011904761904762</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -2654,6 +3090,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.1071428571428571</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -2668,6 +3107,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.03571428571428571</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -2680,6 +3122,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2693,6 +3138,9 @@
       </c>
       <c r="D10" t="n">
         <v>94.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9999999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2706,7 +3154,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2731,6 +3179,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -2745,6 +3198,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -2759,6 +3215,9 @@
       <c r="D3" t="n">
         <v>152</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.608</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -2773,6 +3232,9 @@
       <c r="D4" t="n">
         <v>32.25</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.172</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -2787,6 +3249,9 @@
       <c r="D5" t="n">
         <v>8</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.064</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -2801,6 +3266,9 @@
       <c r="D6" t="n">
         <v>2.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -2815,6 +3283,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.07199999999999999</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -2829,6 +3300,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.032</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -2841,6 +3315,9 @@
         <v>3</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0.012</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2854,6 +3331,9 @@
       </c>
       <c r="D10" t="n">
         <v>194.75</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2867,7 +3347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2892,6 +3372,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -2906,6 +3391,9 @@
       <c r="D2" t="n">
         <v>13</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.06018518518518518</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -2920,6 +3408,9 @@
       <c r="D3" t="n">
         <v>60</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.2777777777777778</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -2934,6 +3425,9 @@
       <c r="D4" t="n">
         <v>51</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.3148148148148148</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -2948,6 +3442,9 @@
       <c r="D5" t="n">
         <v>16.5</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1527777777777778</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -2962,6 +3459,9 @@
       <c r="D6" t="n">
         <v>1</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.01851851851851852</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -2976,6 +3476,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.08333333333333333</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -2990,6 +3493,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.09259259259259259</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -3002,6 +3508,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3015,6 +3524,9 @@
       </c>
       <c r="D10" t="n">
         <v>141.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3028,7 +3540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3053,6 +3565,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -3067,6 +3584,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -3081,6 +3601,9 @@
       <c r="D3" t="n">
         <v>44</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.1981981981981982</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -3095,6 +3618,9 @@
       <c r="D4" t="n">
         <v>67.5</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.4054054054054054</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -3109,6 +3635,9 @@
       <c r="D5" t="n">
         <v>17.5</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1576576576576577</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -3123,6 +3652,9 @@
       <c r="D6" t="n">
         <v>4</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.07207207207207207</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -3137,6 +3669,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.1216216216216216</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -3151,6 +3686,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.04504504504504504</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -3163,6 +3701,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3176,6 +3717,9 @@
       </c>
       <c r="D10" t="n">
         <v>133</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3189,7 +3733,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3214,6 +3758,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -3228,6 +3777,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -3242,6 +3794,9 @@
       <c r="D3" t="n">
         <v>32</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.1904761904761905</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -3256,6 +3811,9 @@
       <c r="D4" t="n">
         <v>32.25</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.2559523809523809</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -3270,6 +3828,9 @@
       <c r="D5" t="n">
         <v>26</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.3095238095238095</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -3284,6 +3845,9 @@
       <c r="D6" t="n">
         <v>4.25</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.1011904761904762</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -3298,6 +3862,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.1071428571428571</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -3312,6 +3879,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.03571428571428571</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -3324,6 +3894,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3337,6 +3910,9 @@
       </c>
       <c r="D10" t="n">
         <v>94.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9999999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3350,7 +3926,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3375,6 +3951,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -3389,6 +3970,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -3403,6 +3987,9 @@
       <c r="D3" t="n">
         <v>60</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.2678571428571428</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -3417,6 +4004,9 @@
       <c r="D4" t="n">
         <v>72</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.4285714285714285</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -3431,6 +4021,9 @@
       <c r="D5" t="n">
         <v>10</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.08928571428571429</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -3445,6 +4038,9 @@
       <c r="D6" t="n">
         <v>5.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.09821428571428571</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -3459,6 +4055,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.1160714285714286</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -3473,6 +4072,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -3485,6 +4087,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3498,6 +4103,9 @@
       </c>
       <c r="D10" t="n">
         <v>147.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3511,7 +4119,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3536,6 +4144,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -3550,6 +4163,9 @@
       <c r="D2" t="n">
         <v>18</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.07725321888412018</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -3564,6 +4180,9 @@
       <c r="D3" t="n">
         <v>51</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.2188841201716738</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -3578,6 +4197,9 @@
       <c r="D4" t="n">
         <v>75</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.4291845493562232</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -3592,6 +4214,9 @@
       <c r="D5" t="n">
         <v>13.5</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1158798283261803</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -3606,6 +4231,9 @@
       <c r="D6" t="n">
         <v>3.75</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.06437768240343347</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -3620,6 +4248,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.05150214592274678</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -3634,6 +4265,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.04291845493562232</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -3646,6 +4280,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3659,6 +4296,9 @@
       </c>
       <c r="D10" t="n">
         <v>161.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3672,7 +4312,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3697,6 +4337,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -3711,6 +4356,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -3725,6 +4373,9 @@
       <c r="D3" t="n">
         <v>100</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.3875968992248062</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -3739,6 +4390,9 @@
       <c r="D4" t="n">
         <v>53.25</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.2751937984496124</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -3753,6 +4407,9 @@
       <c r="D5" t="n">
         <v>15.5</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1201550387596899</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -3767,6 +4424,9 @@
       <c r="D6" t="n">
         <v>3.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.05426356589147287</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -3781,6 +4441,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.124031007751938</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -3795,6 +4458,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.03875968992248062</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -3807,6 +4473,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3820,6 +4489,9 @@
       </c>
       <c r="D10" t="n">
         <v>172.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3833,7 +4505,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3858,6 +4530,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -3872,6 +4549,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -3886,6 +4566,9 @@
       <c r="D3" t="n">
         <v>97</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.4008264462809917</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -3900,6 +4583,9 @@
       <c r="D4" t="n">
         <v>36.75</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.2024793388429752</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -3914,6 +4600,9 @@
       <c r="D5" t="n">
         <v>11</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.09090909090909091</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -3928,6 +4617,9 @@
       <c r="D6" t="n">
         <v>2.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.04132231404958678</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -3942,6 +4634,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.2148760330578512</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -3956,6 +4651,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.04958677685950413</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -3968,6 +4666,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3981,6 +4682,9 @@
       </c>
       <c r="D10" t="n">
         <v>147.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3994,7 +4698,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4019,6 +4723,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -4033,6 +4742,9 @@
       <c r="D2" t="n">
         <v>21</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.09130434782608696</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -4047,6 +4759,9 @@
       <c r="D3" t="n">
         <v>64</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.2782608695652174</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -4061,6 +4776,9 @@
       <c r="D4" t="n">
         <v>59.25</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.3434782608695652</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -4075,6 +4793,9 @@
       <c r="D5" t="n">
         <v>9.5</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.08260869565217391</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -4089,6 +4810,9 @@
       <c r="D6" t="n">
         <v>4</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.06956521739130435</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -4103,6 +4827,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.08260869565217391</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -4117,6 +4844,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.05217391304347826</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -4129,6 +4859,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -4142,6 +4875,9 @@
       </c>
       <c r="D10" t="n">
         <v>157.75</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4155,7 +4891,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4180,6 +4916,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -4194,6 +4935,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -4208,6 +4952,9 @@
       <c r="D3" t="n">
         <v>55</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.2217741935483871</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -4222,6 +4969,9 @@
       <c r="D4" t="n">
         <v>62.25</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.3346774193548387</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -4236,6 +4986,9 @@
       <c r="D5" t="n">
         <v>12.5</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1008064516129032</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -4250,6 +5003,9 @@
       <c r="D6" t="n">
         <v>8.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.1370967741935484</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -4264,6 +5020,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.1733870967741936</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -4278,6 +5037,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.03225806451612903</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -4290,6 +5052,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -4303,6 +5068,9 @@
       </c>
       <c r="D10" t="n">
         <v>138.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4316,7 +5084,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4341,6 +5109,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -4355,6 +5128,9 @@
       <c r="D2" t="n">
         <v>10</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.04201680672268908</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -4369,6 +5145,9 @@
       <c r="D3" t="n">
         <v>81</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.3403361344537815</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -4383,6 +5162,9 @@
       <c r="D4" t="n">
         <v>77.25</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.4327731092436975</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -4397,6 +5179,9 @@
       <c r="D5" t="n">
         <v>4</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.03361344537815126</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -4411,6 +5196,9 @@
       <c r="D6" t="n">
         <v>1.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.02521008403361345</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -4425,6 +5213,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.06722689075630252</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -4439,6 +5230,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.05882352941176471</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -4451,6 +5245,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -4464,6 +5261,9 @@
       </c>
       <c r="D10" t="n">
         <v>173.75</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4477,7 +5277,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4502,6 +5302,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -4516,6 +5321,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -4530,6 +5338,9 @@
       <c r="D3" t="n">
         <v>147</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.6282051282051282</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -4544,6 +5355,9 @@
       <c r="D4" t="n">
         <v>25.5</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.1452991452991453</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -4558,6 +5372,9 @@
       <c r="D5" t="n">
         <v>7</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.05982905982905983</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -4572,6 +5389,9 @@
       <c r="D6" t="n">
         <v>2.5</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.04273504273504274</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -4586,6 +5406,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.08974358974358974</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -4600,6 +5423,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.03418803418803419</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -4612,6 +5438,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -4625,6 +5454,9 @@
       </c>
       <c r="D10" t="n">
         <v>182</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4638,7 +5470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4663,6 +5495,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -4677,6 +5514,9 @@
       <c r="D2" t="n">
         <v>17</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.07327586206896551</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -4691,6 +5531,9 @@
       <c r="D3" t="n">
         <v>85</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.3663793103448276</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -4705,6 +5548,9 @@
       <c r="D4" t="n">
         <v>41.25</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.2370689655172414</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -4719,6 +5565,9 @@
       <c r="D5" t="n">
         <v>13.5</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1163793103448276</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -4733,6 +5582,9 @@
       <c r="D6" t="n">
         <v>3</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.05172413793103448</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -4747,6 +5599,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.09482758620689655</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -4761,6 +5616,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.0603448275862069</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -4773,6 +5631,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -4786,6 +5647,9 @@
       </c>
       <c r="D10" t="n">
         <v>159.75</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4799,7 +5663,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4824,6 +5688,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>%-age</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -4838,6 +5707,9 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -4852,6 +5724,9 @@
       <c r="D3" t="n">
         <v>50</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.2136752136752137</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -4866,6 +5741,9 @@
       <c r="D4" t="n">
         <v>60</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.3418803418803419</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -4880,6 +5758,9 @@
       <c r="D5" t="n">
         <v>14.5</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.1239316239316239</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -4894,6 +5775,9 @@
       <c r="D6" t="n">
         <v>5.75</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.09829059829059829</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -4908,6 +5792,9 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.1709401709401709</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -4922,6 +5809,9 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.05128205128205128</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -4934,6 +5824,9 @@
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -4947,6 +5840,9 @@
       </c>
       <c r="D10" t="n">
         <v>130.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>